<commit_message>
still work on cursach
</commit_message>
<xml_diff>
--- a/dm/curs1.xlsx
+++ b/dm/curs1.xlsx
@@ -5,19 +5,20 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kupp\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kupp\Documents\itmo_labs\dm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E540CDC-1EC0-47DE-BF34-687350F31B65}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A43711F-21CB-48CE-A848-A4C66E990D24}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10815" yWindow="5430" windowWidth="10785" windowHeight="9375" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6975" yWindow="2025" windowWidth="10785" windowHeight="9375" firstSheet="4" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Табл Ист" sheetId="1" r:id="rId1"/>
     <sheet name="Максимальные кубы" sheetId="2" r:id="rId2"/>
     <sheet name="Импликантая таблица" sheetId="3" r:id="rId3"/>
     <sheet name="привед" sheetId="4" state="hidden" r:id="rId4"/>
-    <sheet name="Привед1" sheetId="6" r:id="rId5"/>
+    <sheet name="Привед Имл Табл" sheetId="6" r:id="rId5"/>
+    <sheet name="Карты Гавно" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="127">
   <si>
     <t>N</t>
   </si>
@@ -870,12 +871,165 @@
   <si>
     <t>J</t>
   </si>
+  <si>
+    <r>
+      <t>X</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>X</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>5</t>
+    </r>
+  </si>
+  <si>
+    <t>00</t>
+  </si>
+  <si>
+    <t>01</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <r>
+      <t>X</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>X</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>X</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = 0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>X</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = 1</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -980,6 +1134,15 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <vertAlign val="subscript"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -994,7 +1157,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="34">
     <border>
       <left/>
       <right/>
@@ -1149,12 +1312,286 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -1171,14 +1608,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment textRotation="255"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1"/>
+    <xf numFmtId="49" fontId="11" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1187,20 +1638,11 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment textRotation="255"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment textRotation="255"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1220,11 +1662,48 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1"/>
-    <xf numFmtId="49" fontId="11" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment textRotation="255"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Вывод" xfId="1" builtinId="21"/>
@@ -1508,8 +1987,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="H33" sqref="H33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1587,7 +2066,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="2" t="str">
-        <f t="shared" ref="B3:B34" si="0">DEC2BIN(A3,5)</f>
+        <f t="shared" ref="B3:B33" si="0">DEC2BIN(A3,5)</f>
         <v>00001</v>
       </c>
       <c r="C3" s="2" t="str">
@@ -1805,7 +2284,7 @@
         <v>7</v>
       </c>
       <c r="G9" s="2">
-        <f t="shared" si="5"/>
+        <f>D9+F9</f>
         <v>7</v>
       </c>
       <c r="H9" s="2">
@@ -2619,8 +3098,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3661A5AE-718B-4B1A-B8C2-77CD58073A74}">
   <dimension ref="A1:L27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13:J27"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:L27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2638,26 +3117,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="24" t="s">
         <v>99</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="19" t="s">
+      <c r="B1" s="26"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="24" t="s">
         <v>100</v>
       </c>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="19" t="s">
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="24" t="s">
         <v>101</v>
       </c>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
-      <c r="K1" s="19" t="s">
+      <c r="I1" s="27"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="24" t="s">
         <v>98</v>
       </c>
-      <c r="L1" s="22"/>
+      <c r="L1" s="25"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
@@ -3051,11 +3530,11 @@
       <c r="G12" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="H12" s="16" t="s">
+      <c r="H12" s="22" t="s">
         <v>97</v>
       </c>
-      <c r="I12" s="17"/>
-      <c r="J12" s="17"/>
+      <c r="I12" s="23"/>
+      <c r="J12" s="37"/>
       <c r="K12" s="3">
         <v>11</v>
       </c>
@@ -3146,7 +3625,7 @@
       <c r="K15" s="5">
         <v>14</v>
       </c>
-      <c r="L15" s="18" t="s">
+      <c r="L15" s="16" t="s">
         <v>88</v>
       </c>
     </row>
@@ -3369,7 +3848,7 @@
   <dimension ref="A1:Q16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Q10" sqref="Q10"/>
+      <selection sqref="A1:P16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3379,152 +3858,152 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="28" t="s">
         <v>103</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="25" t="s">
+      <c r="B1" s="28"/>
+      <c r="C1" s="29" t="s">
         <v>102</v>
       </c>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
-      <c r="L1" s="25"/>
-      <c r="M1" s="25"/>
-      <c r="N1" s="25"/>
-      <c r="O1" s="25"/>
-      <c r="P1" s="25"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
+      <c r="L1" s="29"/>
+      <c r="M1" s="29"/>
+      <c r="N1" s="29"/>
+      <c r="O1" s="29"/>
+      <c r="P1" s="29"/>
       <c r="Q1" s="12"/>
     </row>
     <row r="2" spans="1:17" ht="76.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="24"/>
-      <c r="B2" s="24"/>
-      <c r="C2" s="34" t="s">
+      <c r="A2" s="28"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="26" t="s">
+      <c r="D2" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="26" t="s">
+      <c r="E2" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="34" t="s">
+      <c r="F2" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="26" t="s">
+      <c r="G2" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="26" t="s">
+      <c r="H2" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="26" t="s">
+      <c r="I2" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="J2" s="34" t="s">
+      <c r="J2" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="K2" s="26" t="s">
+      <c r="K2" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="L2" s="26" t="s">
+      <c r="L2" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="M2" s="26" t="s">
+      <c r="M2" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="N2" s="26" t="s">
+      <c r="N2" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="O2" s="26" t="s">
+      <c r="O2" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="P2" s="26" t="s">
+      <c r="P2" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="Q2" s="23"/>
+      <c r="Q2" s="17"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="33">
+      <c r="A3" s="19">
         <v>1</v>
       </c>
-      <c r="B3" s="33" t="s">
+      <c r="B3" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="35" t="s">
+      <c r="C3" s="21" t="s">
         <v>104</v>
       </c>
-      <c r="D3" s="33" t="s">
-        <v>105</v>
-      </c>
-      <c r="E3" s="33"/>
-      <c r="F3" s="33"/>
-      <c r="G3" s="33"/>
-      <c r="H3" s="33"/>
-      <c r="I3" s="33"/>
-      <c r="J3" s="33"/>
-      <c r="K3" s="33"/>
-      <c r="L3" s="33"/>
-      <c r="M3" s="33"/>
-      <c r="N3" s="33"/>
-      <c r="O3" s="33"/>
-      <c r="P3" s="33"/>
+      <c r="D3" s="19" t="s">
+        <v>105</v>
+      </c>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
+      <c r="K3" s="19"/>
+      <c r="L3" s="19"/>
+      <c r="M3" s="19"/>
+      <c r="N3" s="19"/>
+      <c r="O3" s="19"/>
+      <c r="P3" s="19"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="33">
+      <c r="A4" s="19">
         <v>2</v>
       </c>
-      <c r="B4" s="33" t="s">
+      <c r="B4" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="35" t="s">
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="21" t="s">
         <v>104</v>
       </c>
-      <c r="G4" s="33" t="s">
-        <v>105</v>
-      </c>
-      <c r="H4" s="33"/>
-      <c r="I4" s="33"/>
-      <c r="J4" s="33"/>
-      <c r="K4" s="33"/>
-      <c r="L4" s="33"/>
-      <c r="M4" s="33"/>
-      <c r="N4" s="33"/>
-      <c r="O4" s="33"/>
-      <c r="P4" s="33"/>
+      <c r="G4" s="19" t="s">
+        <v>105</v>
+      </c>
+      <c r="H4" s="19"/>
+      <c r="I4" s="19"/>
+      <c r="J4" s="19"/>
+      <c r="K4" s="19"/>
+      <c r="L4" s="19"/>
+      <c r="M4" s="19"/>
+      <c r="N4" s="19"/>
+      <c r="O4" s="19"/>
+      <c r="P4" s="19"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" s="33">
+      <c r="A5" s="19">
         <v>3</v>
       </c>
-      <c r="B5" s="33" t="s">
+      <c r="B5" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="C5" s="33"/>
-      <c r="D5" s="33"/>
-      <c r="E5" s="33"/>
-      <c r="F5" s="33"/>
-      <c r="G5" s="33"/>
-      <c r="H5" s="33"/>
-      <c r="I5" s="33"/>
-      <c r="J5" s="35" t="s">
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="19"/>
+      <c r="I5" s="19"/>
+      <c r="J5" s="21" t="s">
         <v>104</v>
       </c>
-      <c r="K5" s="33"/>
-      <c r="L5" s="33"/>
-      <c r="M5" s="33"/>
-      <c r="N5" s="33" t="s">
-        <v>105</v>
-      </c>
-      <c r="O5" s="33"/>
-      <c r="P5" s="33"/>
+      <c r="K5" s="19"/>
+      <c r="L5" s="19"/>
+      <c r="M5" s="19"/>
+      <c r="N5" s="19" t="s">
+        <v>105</v>
+      </c>
+      <c r="O5" s="19"/>
+      <c r="P5" s="19"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
@@ -3533,14 +4012,14 @@
       <c r="B6" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C6" s="33"/>
+      <c r="C6" s="19"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
-      <c r="F6" s="33"/>
+      <c r="F6" s="19"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
-      <c r="J6" s="33"/>
+      <c r="J6" s="19"/>
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
       <c r="M6" s="2" t="s">
@@ -3559,14 +4038,14 @@
       <c r="B7" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C7" s="33"/>
+      <c r="C7" s="19"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
-      <c r="F7" s="33"/>
+      <c r="F7" s="19"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
-      <c r="J7" s="33"/>
+      <c r="J7" s="19"/>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
       <c r="M7" s="2" t="s">
@@ -3583,14 +4062,14 @@
       <c r="B8" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="C8" s="33"/>
+      <c r="C8" s="19"/>
       <c r="D8" s="2" t="s">
         <v>105</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="F8" s="33"/>
+      <c r="F8" s="19"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2" t="s">
         <v>105</v>
@@ -3598,7 +4077,7 @@
       <c r="I8" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="J8" s="33"/>
+      <c r="J8" s="19"/>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
@@ -3613,18 +4092,18 @@
       <c r="B9" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="C9" s="33"/>
+      <c r="C9" s="19"/>
       <c r="D9" s="2" t="s">
         <v>105</v>
       </c>
       <c r="E9" s="2"/>
-      <c r="F9" s="33"/>
+      <c r="F9" s="19"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2" t="s">
         <v>105</v>
       </c>
       <c r="I9" s="2"/>
-      <c r="J9" s="33"/>
+      <c r="J9" s="19"/>
       <c r="K9" s="2"/>
       <c r="L9" s="2" t="s">
         <v>105</v>
@@ -3643,18 +4122,18 @@
       <c r="B10" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="C10" s="33"/>
+      <c r="C10" s="19"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="F10" s="33"/>
+      <c r="F10" s="19"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
       <c r="I10" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="J10" s="33"/>
+      <c r="J10" s="19"/>
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
       <c r="M10" s="2"/>
@@ -3663,26 +4142,26 @@
       <c r="P10" s="2"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" s="33">
+      <c r="A11" s="19">
         <v>9</v>
       </c>
-      <c r="B11" s="33" t="s">
+      <c r="B11" s="19" t="s">
         <v>83</v>
       </c>
-      <c r="C11" s="33"/>
-      <c r="D11" s="33"/>
-      <c r="E11" s="33"/>
-      <c r="F11" s="33"/>
-      <c r="G11" s="33"/>
-      <c r="H11" s="33"/>
-      <c r="I11" s="33"/>
-      <c r="J11" s="33"/>
-      <c r="K11" s="33"/>
-      <c r="L11" s="33"/>
-      <c r="M11" s="33"/>
-      <c r="N11" s="33"/>
-      <c r="O11" s="33"/>
-      <c r="P11" s="33"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="19"/>
+      <c r="H11" s="19"/>
+      <c r="I11" s="19"/>
+      <c r="J11" s="19"/>
+      <c r="K11" s="19"/>
+      <c r="L11" s="19"/>
+      <c r="M11" s="19"/>
+      <c r="N11" s="19"/>
+      <c r="O11" s="19"/>
+      <c r="P11" s="19"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
@@ -3691,10 +4170,10 @@
       <c r="B12" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="C12" s="33"/>
+      <c r="C12" s="19"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
-      <c r="F12" s="33"/>
+      <c r="F12" s="19"/>
       <c r="G12" s="2" t="s">
         <v>105</v>
       </c>
@@ -3704,7 +4183,7 @@
       <c r="I12" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="J12" s="33"/>
+      <c r="J12" s="19"/>
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
       <c r="M12" s="2"/>
@@ -3719,10 +4198,10 @@
       <c r="B13" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C13" s="33"/>
+      <c r="C13" s="19"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
-      <c r="F13" s="33"/>
+      <c r="F13" s="19"/>
       <c r="G13" s="2" t="s">
         <v>105</v>
       </c>
@@ -3730,7 +4209,7 @@
         <v>105</v>
       </c>
       <c r="I13" s="2"/>
-      <c r="J13" s="33"/>
+      <c r="J13" s="19"/>
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
@@ -3749,16 +4228,16 @@
       <c r="B14" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="C14" s="33"/>
+      <c r="C14" s="19"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
-      <c r="F14" s="33"/>
+      <c r="F14" s="19"/>
       <c r="G14" s="2" t="s">
         <v>105</v>
       </c>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
-      <c r="J14" s="33"/>
+      <c r="J14" s="19"/>
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
       <c r="M14" s="2"/>
@@ -3775,14 +4254,14 @@
       <c r="B15" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="C15" s="33"/>
+      <c r="C15" s="19"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
-      <c r="F15" s="33"/>
+      <c r="F15" s="19"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
-      <c r="J15" s="33"/>
+      <c r="J15" s="19"/>
       <c r="K15" s="2" t="s">
         <v>105</v>
       </c>
@@ -3805,14 +4284,14 @@
       <c r="B16" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="C16" s="33"/>
+      <c r="C16" s="19"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
-      <c r="F16" s="33"/>
+      <c r="F16" s="19"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
-      <c r="J16" s="33"/>
+      <c r="J16" s="19"/>
       <c r="K16" s="2" t="s">
         <v>105</v>
       </c>
@@ -3855,7 +4334,7 @@
   <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3866,52 +4345,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="30" t="s">
         <v>103</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="25" t="s">
+      <c r="B1" s="31"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="29" t="s">
         <v>102</v>
       </c>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
       <c r="L1" s="12"/>
     </row>
     <row r="2" spans="1:12" ht="76.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="30"/>
-      <c r="B2" s="31"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="26" t="s">
+      <c r="A2" s="33"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="26" t="s">
+      <c r="E2" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="26" t="s">
+      <c r="F2" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="26" t="s">
+      <c r="G2" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="26" t="s">
+      <c r="H2" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="26" t="s">
+      <c r="I2" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="J2" s="26" t="s">
+      <c r="J2" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="K2" s="26" t="s">
+      <c r="K2" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="L2" s="23"/>
+      <c r="L2" s="17"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
@@ -4157,4 +4636,408 @@
     <ignoredError sqref="D2:K2" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C6E4DEA-54E3-4A20-83E2-E03EE642AE6F}">
+  <dimension ref="A1:N15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O7" sqref="O7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="6" width="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="13" width="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+      <c r="C1" s="38" t="s">
+        <v>116</v>
+      </c>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="J1" s="38" t="s">
+        <v>116</v>
+      </c>
+      <c r="K1" s="38"/>
+      <c r="L1" s="38"/>
+      <c r="M1" s="38"/>
+      <c r="N1" s="40"/>
+    </row>
+    <row r="2" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="16"/>
+      <c r="C2" s="41" t="s">
+        <v>117</v>
+      </c>
+      <c r="D2" s="44" t="s">
+        <v>118</v>
+      </c>
+      <c r="E2" s="41" t="s">
+        <v>119</v>
+      </c>
+      <c r="F2" s="41" t="s">
+        <v>120</v>
+      </c>
+      <c r="I2" s="16"/>
+      <c r="J2" s="41" t="s">
+        <v>117</v>
+      </c>
+      <c r="K2" s="41" t="s">
+        <v>118</v>
+      </c>
+      <c r="L2" s="44" t="s">
+        <v>119</v>
+      </c>
+      <c r="M2" s="41" t="s">
+        <v>120</v>
+      </c>
+      <c r="N2" s="40"/>
+    </row>
+    <row r="3" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="39" t="s">
+        <v>124</v>
+      </c>
+      <c r="B3" s="41" t="s">
+        <v>117</v>
+      </c>
+      <c r="C3" s="42"/>
+      <c r="D3" s="52" t="s">
+        <v>122</v>
+      </c>
+      <c r="E3" s="50"/>
+      <c r="F3" s="41"/>
+      <c r="H3" s="39" t="s">
+        <v>124</v>
+      </c>
+      <c r="I3" s="41" t="s">
+        <v>117</v>
+      </c>
+      <c r="J3" s="44"/>
+      <c r="K3" s="56"/>
+      <c r="L3" s="53" t="s">
+        <v>122</v>
+      </c>
+      <c r="M3" s="43"/>
+      <c r="N3" s="40"/>
+    </row>
+    <row r="4" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="39"/>
+      <c r="B4" s="41" t="s">
+        <v>118</v>
+      </c>
+      <c r="C4" s="56"/>
+      <c r="D4" s="53" t="s">
+        <v>122</v>
+      </c>
+      <c r="E4" s="51" t="s">
+        <v>122</v>
+      </c>
+      <c r="F4" s="43" t="s">
+        <v>123</v>
+      </c>
+      <c r="H4" s="39"/>
+      <c r="I4" s="42" t="s">
+        <v>118</v>
+      </c>
+      <c r="J4" s="46" t="s">
+        <v>122</v>
+      </c>
+      <c r="K4" s="47" t="s">
+        <v>122</v>
+      </c>
+      <c r="L4" s="55"/>
+      <c r="M4" s="41" t="s">
+        <v>123</v>
+      </c>
+      <c r="N4" s="40"/>
+    </row>
+    <row r="5" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="39"/>
+      <c r="B5" s="42" t="s">
+        <v>119</v>
+      </c>
+      <c r="C5" s="57" t="s">
+        <v>122</v>
+      </c>
+      <c r="D5" s="54" t="s">
+        <v>122</v>
+      </c>
+      <c r="E5" s="49" t="s">
+        <v>122</v>
+      </c>
+      <c r="F5" s="43" t="s">
+        <v>123</v>
+      </c>
+      <c r="H5" s="39"/>
+      <c r="I5" s="42" t="s">
+        <v>119</v>
+      </c>
+      <c r="J5" s="48" t="s">
+        <v>122</v>
+      </c>
+      <c r="K5" s="49" t="s">
+        <v>122</v>
+      </c>
+      <c r="L5" s="50"/>
+      <c r="M5" s="44" t="s">
+        <v>123</v>
+      </c>
+      <c r="N5" s="40"/>
+    </row>
+    <row r="6" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="39"/>
+      <c r="B6" s="42" t="s">
+        <v>120</v>
+      </c>
+      <c r="C6" s="58" t="s">
+        <v>122</v>
+      </c>
+      <c r="D6" s="55"/>
+      <c r="E6" s="45"/>
+      <c r="F6" s="41"/>
+      <c r="H6" s="39"/>
+      <c r="I6" s="41" t="s">
+        <v>120</v>
+      </c>
+      <c r="J6" s="45"/>
+      <c r="K6" s="59"/>
+      <c r="L6" s="60" t="s">
+        <v>122</v>
+      </c>
+      <c r="M6" s="61" t="s">
+        <v>122</v>
+      </c>
+      <c r="N6" s="40"/>
+    </row>
+    <row r="7" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+      <c r="A7" s="38" t="s">
+        <v>125</v>
+      </c>
+      <c r="B7" s="38"/>
+      <c r="C7" s="38"/>
+      <c r="D7" s="38"/>
+      <c r="E7" s="38"/>
+      <c r="F7" s="38"/>
+      <c r="H7" s="38" t="s">
+        <v>126</v>
+      </c>
+      <c r="I7" s="38"/>
+      <c r="J7" s="38"/>
+      <c r="K7" s="38"/>
+      <c r="L7" s="38"/>
+      <c r="M7" s="38"/>
+      <c r="N7" s="40"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="H8" s="40"/>
+      <c r="I8" s="40"/>
+      <c r="J8" s="40"/>
+      <c r="K8" s="40"/>
+      <c r="L8" s="40"/>
+      <c r="M8" s="40"/>
+      <c r="N8" s="40"/>
+    </row>
+    <row r="9" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+      <c r="C9" s="38" t="s">
+        <v>116</v>
+      </c>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
+      <c r="J9" s="38" t="s">
+        <v>116</v>
+      </c>
+      <c r="K9" s="38"/>
+      <c r="L9" s="38"/>
+      <c r="M9" s="38"/>
+      <c r="N9" s="40"/>
+    </row>
+    <row r="10" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="16"/>
+      <c r="C10" s="44" t="s">
+        <v>117</v>
+      </c>
+      <c r="D10" s="44" t="s">
+        <v>118</v>
+      </c>
+      <c r="E10" s="44" t="s">
+        <v>119</v>
+      </c>
+      <c r="F10" s="44" t="s">
+        <v>120</v>
+      </c>
+      <c r="I10" s="16"/>
+      <c r="J10" s="44" t="s">
+        <v>117</v>
+      </c>
+      <c r="K10" s="44" t="s">
+        <v>118</v>
+      </c>
+      <c r="L10" s="44" t="s">
+        <v>119</v>
+      </c>
+      <c r="M10" s="44" t="s">
+        <v>120</v>
+      </c>
+      <c r="N10" s="40"/>
+    </row>
+    <row r="11" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="39" t="s">
+        <v>124</v>
+      </c>
+      <c r="B11" s="42" t="s">
+        <v>117</v>
+      </c>
+      <c r="C11" s="53" t="s">
+        <v>121</v>
+      </c>
+      <c r="D11" s="63"/>
+      <c r="E11" s="62" t="s">
+        <v>121</v>
+      </c>
+      <c r="F11" s="53" t="s">
+        <v>121</v>
+      </c>
+      <c r="H11" s="39" t="s">
+        <v>124</v>
+      </c>
+      <c r="I11" s="42" t="s">
+        <v>117</v>
+      </c>
+      <c r="J11" s="60" t="s">
+        <v>121</v>
+      </c>
+      <c r="K11" s="61" t="s">
+        <v>121</v>
+      </c>
+      <c r="L11" s="65"/>
+      <c r="M11" s="52" t="s">
+        <v>121</v>
+      </c>
+      <c r="N11" s="40"/>
+    </row>
+    <row r="12" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="39"/>
+      <c r="B12" s="42" t="s">
+        <v>118</v>
+      </c>
+      <c r="C12" s="64" t="s">
+        <v>121</v>
+      </c>
+      <c r="D12" s="43"/>
+      <c r="E12" s="59"/>
+      <c r="F12" s="64" t="s">
+        <v>123</v>
+      </c>
+      <c r="H12" s="39"/>
+      <c r="I12" s="42" t="s">
+        <v>118</v>
+      </c>
+      <c r="J12" s="45"/>
+      <c r="K12" s="59"/>
+      <c r="L12" s="66" t="s">
+        <v>121</v>
+      </c>
+      <c r="M12" s="57" t="s">
+        <v>123</v>
+      </c>
+      <c r="N12" s="40"/>
+    </row>
+    <row r="13" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="39"/>
+      <c r="B13" s="42" t="s">
+        <v>119</v>
+      </c>
+      <c r="C13" s="45"/>
+      <c r="D13" s="44"/>
+      <c r="E13" s="44"/>
+      <c r="F13" s="68" t="s">
+        <v>123</v>
+      </c>
+      <c r="H13" s="39"/>
+      <c r="I13" s="42" t="s">
+        <v>119</v>
+      </c>
+      <c r="J13" s="44"/>
+      <c r="K13" s="56"/>
+      <c r="L13" s="67" t="s">
+        <v>121</v>
+      </c>
+      <c r="M13" s="58" t="s">
+        <v>123</v>
+      </c>
+      <c r="N13" s="40"/>
+    </row>
+    <row r="14" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="39"/>
+      <c r="B14" s="42" t="s">
+        <v>120</v>
+      </c>
+      <c r="C14" s="42"/>
+      <c r="D14" s="62" t="s">
+        <v>121</v>
+      </c>
+      <c r="E14" s="53" t="s">
+        <v>121</v>
+      </c>
+      <c r="F14" s="69" t="s">
+        <v>121</v>
+      </c>
+      <c r="H14" s="39"/>
+      <c r="I14" s="42" t="s">
+        <v>120</v>
+      </c>
+      <c r="J14" s="60" t="s">
+        <v>121</v>
+      </c>
+      <c r="K14" s="61" t="s">
+        <v>121</v>
+      </c>
+      <c r="L14" s="6"/>
+      <c r="M14" s="64"/>
+    </row>
+    <row r="15" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+      <c r="A15" s="38" t="s">
+        <v>125</v>
+      </c>
+      <c r="B15" s="38"/>
+      <c r="C15" s="38"/>
+      <c r="D15" s="38"/>
+      <c r="E15" s="38"/>
+      <c r="F15" s="38"/>
+      <c r="H15" s="38" t="s">
+        <v>126</v>
+      </c>
+      <c r="I15" s="38"/>
+      <c r="J15" s="38"/>
+      <c r="K15" s="38"/>
+      <c r="L15" s="38"/>
+      <c r="M15" s="38"/>
+    </row>
+  </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="J9:M9"/>
+    <mergeCell ref="A11:A14"/>
+    <mergeCell ref="H11:H14"/>
+    <mergeCell ref="A15:F15"/>
+    <mergeCell ref="H15:M15"/>
+    <mergeCell ref="A3:A6"/>
+    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="A7:F7"/>
+    <mergeCell ref="J1:M1"/>
+    <mergeCell ref="H3:H6"/>
+    <mergeCell ref="H7:M7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="C2:F2 C5:F5 J2:M2 M4 L3 J4:J5 K5 L6:M6 B3:B6 I3:I6 D3 D4:F4 C6 K4 C10:M10 B13 B11 B12 B14 G14:I14 G11:I11 F12:I12 C12 D14:F14 L13:M13 C11 E11:F11 L12:M12 J11:K11 J14:K14 M11 F13:I13" numberStoredAsText="1"/>
+  </ignoredErrors>
+</worksheet>
 </file>
</xml_diff>